<commit_message>
mcd and timesheet update
</commit_message>
<xml_diff>
--- a/Timesheet-evaluation.xlsx
+++ b/Timesheet-evaluation.xlsx
@@ -277,7 +277,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -322,12 +322,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -385,7 +379,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,19 +404,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,8 +499,8 @@
   </sheetPr>
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -583,14 +569,16 @@
       <c r="E4" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G4" s="4" t="n">
         <f aca="false">E4-F4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
         <f aca="false">(F4/(F4+G4))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -609,14 +597,16 @@
       <c r="E5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G5" s="4" t="n">
         <f aca="false">E5-F5</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5" t="n">
         <f aca="false">(F5/(F5+G5))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -635,14 +625,16 @@
       <c r="E6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G6" s="4" t="n">
         <f aca="false">E6-F6</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
         <f aca="false">(F6/(F6+G6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -661,14 +653,16 @@
       <c r="E7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G7" s="4" t="n">
         <f aca="false">E7-F7</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
         <f aca="false">(F7/(F7+G7))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -687,14 +681,16 @@
       <c r="E8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G8" s="4" t="n">
         <f aca="false">E8-F8</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
         <f aca="false">(F8/(F8+G8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -713,14 +709,16 @@
       <c r="E9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G9" s="4" t="n">
         <f aca="false">E9-F9</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
         <f aca="false">(F9/(F9+G9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -739,14 +737,16 @@
       <c r="E10" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G10" s="4" t="n">
         <f aca="false">E10-F10</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
         <f aca="false">(F10/(F10+G10))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -765,14 +765,16 @@
       <c r="E11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G11" s="4" t="n">
         <f aca="false">E11-F11</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
         <f aca="false">(F11/(F11+G11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -791,14 +793,16 @@
       <c r="E12" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G12" s="4" t="n">
         <f aca="false">E12-F12</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
         <f aca="false">(F12/(F12+G12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -817,14 +821,16 @@
       <c r="E13" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G13" s="4" t="n">
         <f aca="false">E13-F13</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
         <f aca="false">(F13/(F13+G13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -843,14 +849,16 @@
       <c r="E14" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G14" s="4" t="n">
         <f aca="false">E14-F14</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
         <f aca="false">(F14/(F14+G14))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -869,14 +877,16 @@
       <c r="E15" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G15" s="4" t="n">
         <f aca="false">E15-F15</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
         <f aca="false">(F15/(F15+G15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -895,14 +905,16 @@
       <c r="E16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G16" s="4" t="n">
         <f aca="false">E16-F16</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
         <f aca="false">(F16/(F16+G16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -921,21 +933,23 @@
       <c r="E17" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G17" s="4" t="n">
         <f aca="false">E17-F17</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
         <f aca="false">(F17/(F17+G17))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -947,21 +961,23 @@
       <c r="E18" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="G18" s="4" t="n">
         <f aca="false">E18-F18</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H18" s="5" t="n">
         <f aca="false">(F18/(F18+G18))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -987,7 +1003,7 @@
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1100,10 +1116,10 @@
       <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F24" s="7"/>
+      <c r="E24" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6"/>
       <c r="G24" s="4" t="n">
         <f aca="false">E24-F24</f>
         <v>10</v>
@@ -1117,7 +1133,7 @@
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1126,10 +1142,10 @@
       <c r="D25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F25" s="7"/>
+      <c r="E25" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" s="6"/>
       <c r="G25" s="4" t="n">
         <f aca="false">E25-F25</f>
         <v>10</v>
@@ -1143,7 +1159,7 @@
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1152,10 +1168,10 @@
       <c r="D26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F26" s="7"/>
+      <c r="E26" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="G26" s="4" t="n">
         <f aca="false">E26-F26</f>
         <v>10</v>
@@ -1169,7 +1185,7 @@
       <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1178,10 +1194,10 @@
       <c r="D27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="E27" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" s="6"/>
       <c r="G27" s="4" t="n">
         <f aca="false">E27-F27</f>
         <v>10</v>
@@ -1195,7 +1211,7 @@
       <c r="A28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1204,10 +1220,10 @@
       <c r="D28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F28" s="7"/>
+      <c r="E28" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="4" t="n">
         <f aca="false">E28-F28</f>
         <v>10</v>
@@ -1221,7 +1237,7 @@
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1230,10 +1246,10 @@
       <c r="D29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F29" s="7"/>
+      <c r="E29" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="4" t="n">
         <f aca="false">E29-F29</f>
         <v>10</v>
@@ -1244,100 +1260,106 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="E30" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="G30" s="4" t="n">
         <f aca="false">E30-F30</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30" s="5" t="n">
         <f aca="false">(F30/(F30+G30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="E31" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="G31" s="4" t="n">
         <f aca="false">E31-F31</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" s="5" t="n">
         <f aca="false">(F31/(F31+G31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F32" s="7"/>
+      <c r="E32" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="G32" s="4" t="n">
         <f aca="false">E32-F32</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H32" s="5" t="n">
         <f aca="false">(F32/(F32+G32))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F33" s="7"/>
+      <c r="E33" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F33" s="6"/>
       <c r="G33" s="4" t="n">
         <f aca="false">E33-F33</f>
         <v>5</v>
@@ -1348,22 +1370,22 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F34" s="7"/>
+      <c r="E34" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F34" s="6"/>
       <c r="G34" s="4" t="n">
         <f aca="false">E34-F34</f>
         <v>5</v>
@@ -1374,22 +1396,22 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F35" s="7"/>
+      <c r="E35" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6"/>
       <c r="G35" s="4" t="n">
         <f aca="false">E35-F35</f>
         <v>10</v>
@@ -1400,22 +1422,22 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F36" s="6"/>
       <c r="G36" s="4" t="n">
         <f aca="false">E36-F36</f>
         <v>10</v>
@@ -1426,48 +1448,50 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F37" s="7"/>
+      <c r="E37" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>10</v>
+      </c>
       <c r="G37" s="4" t="n">
         <f aca="false">E37-F37</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H37" s="5" t="n">
         <f aca="false">(F37/(F37+G37))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="7" t="n">
+      <c r="E38" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="4" t="n">
         <f aca="false">E38-F38</f>
         <v>2</v>
@@ -1478,48 +1502,50 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F39" s="7"/>
+      <c r="E39" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="G39" s="4" t="n">
         <f aca="false">E39-F39</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H39" s="5" t="n">
         <f aca="false">(F39/(F39+G39))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="7" t="n">
+      <c r="E40" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="6"/>
       <c r="G40" s="4" t="n">
         <f aca="false">E40-F40</f>
         <v>2</v>
@@ -1530,22 +1556,22 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="7" t="n">
+      <c r="E41" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="4" t="n">
         <f aca="false">E41-F41</f>
         <v>2</v>
@@ -1556,22 +1582,22 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="7" t="n">
+      <c r="E42" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="6"/>
       <c r="G42" s="4" t="n">
         <f aca="false">E42-F42</f>
         <v>2</v>
@@ -1582,22 +1608,22 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="7" t="n">
+      <c r="E43" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="4" t="n">
         <f aca="false">E43-F43</f>
         <v>2</v>
@@ -1608,22 +1634,22 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="7" t="n">
+      <c r="E44" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="4" t="n">
         <f aca="false">E44-F44</f>
         <v>2</v>
@@ -1634,22 +1660,22 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="7" t="n">
+      <c r="E45" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="6"/>
       <c r="G45" s="4" t="n">
         <f aca="false">E45-F45</f>
         <v>2</v>
@@ -1660,22 +1686,22 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="7" t="n">
+      <c r="E46" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="6"/>
       <c r="G46" s="4" t="n">
         <f aca="false">E46-F46</f>
         <v>2</v>
@@ -1686,22 +1712,22 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F47" s="6"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="4" t="n">
         <f aca="false">E47-F47</f>
         <v>2</v>
@@ -1712,22 +1738,22 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F48" s="6"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="4" t="n">
         <f aca="false">E48-F48</f>
         <v>2</v>
@@ -1738,22 +1764,22 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F49" s="6"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="4" t="n">
         <f aca="false">E49-F49</f>
         <v>2</v>
@@ -1764,22 +1790,22 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F50" s="7"/>
+      <c r="E50" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" s="6"/>
       <c r="G50" s="4" t="n">
         <f aca="false">E50-F50</f>
         <v>10</v>
@@ -1790,22 +1816,22 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F51" s="7"/>
+      <c r="E51" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F51" s="6"/>
       <c r="G51" s="4" t="n">
         <f aca="false">E51-F51</f>
         <v>10</v>
@@ -1816,22 +1842,22 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F52" s="7"/>
+      <c r="E52" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F52" s="6"/>
       <c r="G52" s="4" t="n">
         <f aca="false">E52-F52</f>
         <v>10</v>
@@ -1842,22 +1868,22 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F53" s="7"/>
+      <c r="E53" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F53" s="6"/>
       <c r="G53" s="4" t="n">
         <f aca="false">E53-F53</f>
         <v>10</v>
@@ -1868,22 +1894,22 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F54" s="7"/>
+      <c r="E54" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F54" s="6"/>
       <c r="G54" s="4" t="n">
         <f aca="false">E54-F54</f>
         <v>10</v>
@@ -1897,19 +1923,19 @@
       <c r="A55" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F55" s="7"/>
+      <c r="E55" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" s="6"/>
       <c r="G55" s="4" t="n">
         <f aca="false">E55-F55</f>
         <v>10</v>
@@ -1920,22 +1946,22 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F56" s="7"/>
+      <c r="E56" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F56" s="6"/>
       <c r="G56" s="4" t="n">
         <f aca="false">E56-F56</f>
         <v>10</v>
@@ -1946,22 +1972,22 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F57" s="7"/>
+      <c r="E57" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F57" s="6"/>
       <c r="G57" s="4" t="n">
         <f aca="false">E57-F57</f>
         <v>10</v>
@@ -1975,19 +2001,19 @@
       <c r="A58" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F58" s="7"/>
+      <c r="E58" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F58" s="6"/>
       <c r="G58" s="4" t="n">
         <f aca="false">E58-F58</f>
         <v>5</v>
@@ -2001,19 +2027,19 @@
       <c r="A59" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F59" s="7"/>
+      <c r="E59" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" s="6"/>
       <c r="G59" s="4" t="n">
         <f aca="false">E59-F59</f>
         <v>5</v>
@@ -2027,19 +2053,19 @@
       <c r="A60" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F60" s="7"/>
+      <c r="E60" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F60" s="6"/>
       <c r="G60" s="4" t="n">
         <f aca="false">E60-F60</f>
         <v>5</v>
@@ -2056,16 +2082,16 @@
       <c r="B61" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E61" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F61" s="7"/>
+      <c r="E61" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F61" s="6"/>
       <c r="G61" s="4" t="n">
         <f aca="false">E61-F61</f>
         <v>5</v>
@@ -2082,16 +2108,16 @@
       <c r="B62" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E62" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F62" s="6"/>
+      <c r="E62" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F62" s="4"/>
       <c r="G62" s="4" t="n">
         <f aca="false">E62-F62</f>
         <v>5</v>
@@ -2108,16 +2134,16 @@
       <c r="B63" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E63" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F63" s="7"/>
+      <c r="E63" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F63" s="6"/>
       <c r="G63" s="4" t="n">
         <f aca="false">E63-F63</f>
         <v>5</v>
@@ -2134,16 +2160,16 @@
       <c r="B64" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F64" s="7"/>
+      <c r="E64" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F64" s="6"/>
       <c r="G64" s="4" t="n">
         <f aca="false">E64-F64</f>
         <v>5</v>
@@ -2157,19 +2183,19 @@
       <c r="A65" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E65" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F65" s="7"/>
+      <c r="E65" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F65" s="6"/>
       <c r="G65" s="4" t="n">
         <f aca="false">E65-F65</f>
         <v>5</v>
@@ -2183,19 +2209,19 @@
       <c r="A66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E66" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F66" s="7"/>
+      <c r="E66" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F66" s="6"/>
       <c r="G66" s="4" t="n">
         <f aca="false">E66-F66</f>
         <v>5</v>
@@ -2209,19 +2235,19 @@
       <c r="A67" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F67" s="7"/>
+      <c r="E67" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F67" s="6"/>
       <c r="G67" s="4" t="n">
         <f aca="false">E67-F67</f>
         <v>5</v>
@@ -2235,19 +2261,19 @@
       <c r="A68" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F68" s="7"/>
+      <c r="E68" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F68" s="6"/>
       <c r="G68" s="4" t="n">
         <f aca="false">E68-F68</f>
         <v>5</v>
@@ -2261,19 +2287,19 @@
       <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E69" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F69" s="7"/>
+      <c r="E69" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F69" s="6"/>
       <c r="G69" s="4" t="n">
         <f aca="false">E69-F69</f>
         <v>5</v>
@@ -2290,15 +2316,15 @@
       </c>
       <c r="F70" s="4" t="n">
         <f aca="false">SUM(F4:F69)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G70" s="4" t="n">
         <f aca="false">SUM(G4:G69)</f>
-        <v>412</v>
-      </c>
-      <c r="H70" s="10" t="n">
+        <v>307</v>
+      </c>
+      <c r="H70" s="8" t="n">
         <f aca="false">(F70/(F70+G70))</f>
-        <v>0</v>
+        <v>0.254854368932039</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2307,55 +2333,38 @@
       <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="0"/>
-      <c r="C73" s="0"/>
-      <c r="D73" s="0"/>
-      <c r="E73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="2" t="n">
         <f aca="false">E70</f>
         <v>412</v>
       </c>
-      <c r="C74" s="0"/>
-      <c r="D74" s="0"/>
-      <c r="E74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B75" s="2" t="n">
         <f aca="false">F70</f>
-        <v>0</v>
-      </c>
-      <c r="C75" s="0"/>
-      <c r="D75" s="0"/>
-      <c r="E75" s="0"/>
+        <v>105</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="2" t="n">
         <f aca="false">G70</f>
-        <v>412</v>
-      </c>
-      <c r="C76" s="0"/>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
+        <v>307</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0"/>
       <c r="B77" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="0"/>
-      <c r="D77" s="0"/>
-      <c r="E77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3301,7 +3310,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3313,7 +3322,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3321,7 +3330,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3329,7 +3338,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">

</xml_diff>